<commit_message>
Adjust GaugeAreaChart by shifting left
</commit_message>
<xml_diff>
--- a/backend/app/BTIRD.xlsx
+++ b/backend/app/BTIRD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3112FF-36E1-4FA0-B1E3-14D7D1703ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F5081A-C638-4FCC-9E2C-7A67534670ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dell_Report_Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3507" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3507" uniqueCount="145">
   <si>
     <t>op_name</t>
   </si>
@@ -445,9 +445,6 @@
   </si>
   <si>
     <t>23.140.0.2</t>
-  </si>
-  <si>
-    <t>MS</t>
   </si>
   <si>
     <t>BITS007</t>
@@ -873,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,7 +935,7 @@
     <col min="57" max="57" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="9.88671875" customWidth="1"/>
-    <col min="60" max="60" width="31.21875" customWidth="1"/>
+    <col min="60" max="60" width="50" customWidth="1"/>
     <col min="61" max="61" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -1162,7 +1159,7 @@
         <v>45903.424861111111</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2">
         <v>26100.494600000002</v>
@@ -1189,7 +1186,7 @@
         <v>131</v>
       </c>
       <c r="M2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N2" t="s">
         <v>64</v>
@@ -1207,7 +1204,7 @@
         <v>65</v>
       </c>
       <c r="T2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AM2" t="s">
         <v>69</v>
@@ -1265,7 +1262,7 @@
         <v>45903.417870370373</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3">
         <v>26100.494600000002</v>
@@ -1292,7 +1289,7 @@
         <v>131</v>
       </c>
       <c r="M3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N3" t="s">
         <v>64</v>
@@ -1310,7 +1307,7 @@
         <v>65</v>
       </c>
       <c r="T3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM3" t="s">
         <v>68</v>
@@ -1368,7 +1365,7 @@
         <v>45903.717615740738</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4">
         <v>26100.494600000002</v>
@@ -1395,7 +1392,7 @@
         <v>131</v>
       </c>
       <c r="M4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N4" t="s">
         <v>64</v>
@@ -1413,7 +1410,7 @@
         <v>65</v>
       </c>
       <c r="T4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AM4" t="s">
         <v>69</v>
@@ -1471,7 +1468,7 @@
         <v>45903.714965277781</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5">
         <v>26100.494600000002</v>
@@ -1498,7 +1495,7 @@
         <v>131</v>
       </c>
       <c r="M5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N5" t="s">
         <v>64</v>
@@ -1516,7 +1513,7 @@
         <v>65</v>
       </c>
       <c r="T5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM5" t="s">
         <v>68</v>
@@ -1816,7 +1813,7 @@
         <v>45902.417488425926</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8">
         <v>26100.494600000002</v>
@@ -1843,7 +1840,7 @@
         <v>131</v>
       </c>
       <c r="M8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
@@ -1861,7 +1858,7 @@
         <v>65</v>
       </c>
       <c r="T8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM8" t="s">
         <v>68</v>
@@ -1919,7 +1916,7 @@
         <v>45902.422210648147</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9">
         <v>26100.494600000002</v>
@@ -1946,7 +1943,7 @@
         <v>131</v>
       </c>
       <c r="M9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N9" t="s">
         <v>64</v>
@@ -1964,7 +1961,7 @@
         <v>65</v>
       </c>
       <c r="T9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM9" t="s">
         <v>69</v>
@@ -2022,7 +2019,7 @@
         <v>45902.711747685185</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E10">
         <v>26100.494600000002</v>
@@ -2049,7 +2046,7 @@
         <v>131</v>
       </c>
       <c r="M10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N10" t="s">
         <v>64</v>
@@ -2067,7 +2064,7 @@
         <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AM10" t="s">
         <v>69</v>
@@ -2125,7 +2122,7 @@
         <v>45902.701979166668</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11">
         <v>26100.494600000002</v>
@@ -2152,7 +2149,7 @@
         <v>131</v>
       </c>
       <c r="M11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N11" t="s">
         <v>64</v>
@@ -2170,7 +2167,7 @@
         <v>65</v>
       </c>
       <c r="T11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM11" t="s">
         <v>69</v>
@@ -2470,7 +2467,7 @@
         <v>45901.417199074072</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E14">
         <v>26100.494600000002</v>
@@ -2497,7 +2494,7 @@
         <v>131</v>
       </c>
       <c r="M14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N14" t="s">
         <v>64</v>
@@ -2515,7 +2512,7 @@
         <v>65</v>
       </c>
       <c r="T14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM14" t="s">
         <v>68</v>
@@ -2573,7 +2570,7 @@
         <v>45901.420844907407</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15">
         <v>26100.494600000002</v>
@@ -2600,7 +2597,7 @@
         <v>131</v>
       </c>
       <c r="M15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N15" t="s">
         <v>64</v>
@@ -2618,7 +2615,7 @@
         <v>65</v>
       </c>
       <c r="T15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM15" t="s">
         <v>69</v>
@@ -2676,7 +2673,7 @@
         <v>45901.709178240744</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E16">
         <v>26100.494600000002</v>
@@ -2703,7 +2700,7 @@
         <v>131</v>
       </c>
       <c r="M16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N16" t="s">
         <v>64</v>
@@ -2721,7 +2718,7 @@
         <v>65</v>
       </c>
       <c r="T16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM16" t="s">
         <v>68</v>
@@ -2779,7 +2776,7 @@
         <v>45901.715462962966</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17">
         <v>26100.494600000002</v>
@@ -2806,7 +2803,7 @@
         <v>131</v>
       </c>
       <c r="M17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N17" t="s">
         <v>64</v>
@@ -2824,7 +2821,7 @@
         <v>65</v>
       </c>
       <c r="T17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM17" t="s">
         <v>69</v>
@@ -3124,7 +3121,7 @@
         <v>45898.417488425926</v>
       </c>
       <c r="D20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E20">
         <v>26100.494600000002</v>
@@ -3151,7 +3148,7 @@
         <v>131</v>
       </c>
       <c r="M20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N20" t="s">
         <v>64</v>
@@ -3169,7 +3166,7 @@
         <v>65</v>
       </c>
       <c r="T20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM20" t="s">
         <v>69</v>
@@ -3227,7 +3224,7 @@
         <v>45898.417488425926</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21">
         <v>26100.494600000002</v>
@@ -3254,7 +3251,7 @@
         <v>131</v>
       </c>
       <c r="M21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N21" t="s">
         <v>64</v>
@@ -3272,7 +3269,7 @@
         <v>65</v>
       </c>
       <c r="T21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM21" t="s">
         <v>69</v>
@@ -3330,7 +3327,7 @@
         <v>45898.712245370371</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E22">
         <v>26100.494600000002</v>
@@ -3357,7 +3354,7 @@
         <v>131</v>
       </c>
       <c r="M22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N22" t="s">
         <v>64</v>
@@ -3375,7 +3372,7 @@
         <v>65</v>
       </c>
       <c r="T22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM22" t="s">
         <v>69</v>
@@ -3433,7 +3430,7 @@
         <v>45898.707939814813</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23">
         <v>26100.494600000002</v>
@@ -3460,7 +3457,7 @@
         <v>131</v>
       </c>
       <c r="M23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N23" t="s">
         <v>64</v>
@@ -3478,7 +3475,7 @@
         <v>65</v>
       </c>
       <c r="T23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM23" t="s">
         <v>69</v>
@@ -3778,7 +3775,7 @@
         <v>45897.421261574076</v>
       </c>
       <c r="D26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E26">
         <v>26100.494600000002</v>
@@ -3823,7 +3820,7 @@
         <v>65</v>
       </c>
       <c r="T26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM26" t="s">
         <v>69</v>
@@ -3881,7 +3878,7 @@
         <v>45897.702337962961</v>
       </c>
       <c r="D27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E27">
         <v>26100.494600000002</v>
@@ -3926,7 +3923,7 @@
         <v>65</v>
       </c>
       <c r="T27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM27" t="s">
         <v>69</v>
@@ -4226,7 +4223,7 @@
         <v>45896.424131944441</v>
       </c>
       <c r="D30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E30">
         <v>26100.494600000002</v>
@@ -4271,7 +4268,7 @@
         <v>65</v>
       </c>
       <c r="T30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM30" t="s">
         <v>69</v>
@@ -4329,7 +4326,7 @@
         <v>45896.705509259256</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31">
         <v>26100.494600000002</v>
@@ -4374,7 +4371,7 @@
         <v>65</v>
       </c>
       <c r="T31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM31" t="s">
         <v>69</v>
@@ -4674,7 +4671,7 @@
         <v>45895.416851851849</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E34">
         <v>26100.494600000002</v>
@@ -4719,7 +4716,7 @@
         <v>65</v>
       </c>
       <c r="T34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AM34" t="s">
         <v>69</v>
@@ -4777,7 +4774,7 @@
         <v>45895.7109375</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35">
         <v>26100.494600000002</v>
@@ -4822,7 +4819,7 @@
         <v>65</v>
       </c>
       <c r="T35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AM35" t="s">
         <v>69</v>
@@ -4995,7 +4992,7 @@
         <v>45894.422349537039</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E37">
         <v>26100.494600000002</v>
@@ -5040,7 +5037,7 @@
         <v>65</v>
       </c>
       <c r="T37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AM37" t="s">
         <v>69</v>
@@ -5098,7 +5095,7 @@
         <v>45894.715787037036</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E38">
         <v>26100.494600000002</v>
@@ -5143,7 +5140,7 @@
         <v>65</v>
       </c>
       <c r="T38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AM38" t="s">
         <v>69</v>
@@ -5316,7 +5313,7 @@
         <v>45891.417604166665</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E40">
         <v>26100.494600000002</v>
@@ -5361,7 +5358,7 @@
         <v>65</v>
       </c>
       <c r="T40" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="AM40" t="s">
         <v>68</v>
@@ -5422,7 +5419,7 @@
         <v>45891.708703703705</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E41">
         <v>26100.494600000002</v>
@@ -5467,7 +5464,7 @@
         <v>65</v>
       </c>
       <c r="T41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM41" t="s">
         <v>69</v>
@@ -5640,7 +5637,7 @@
         <v>45890.418043981481</v>
       </c>
       <c r="D43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E43">
         <v>26100.494600000002</v>
@@ -5685,7 +5682,7 @@
         <v>65</v>
       </c>
       <c r="T43" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="AM43" t="s">
         <v>68</v>
@@ -5746,7 +5743,7 @@
         <v>45890.7190162037</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E44">
         <v>26100.494600000002</v>
@@ -5791,7 +5788,7 @@
         <v>65</v>
       </c>
       <c r="T44" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="AM44" t="s">
         <v>68</v>
@@ -14436,7 +14433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF5E143-8483-4FCB-BED3-178AEE5EE779}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -14527,7 +14524,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" s="7">
         <v>45901.711516203701</v>
@@ -14542,7 +14539,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="7">
         <v>45901.708333333336</v>

</xml_diff>